<commit_message>
Update Excel to match all regions
</commit_message>
<xml_diff>
--- a/Listado ART.xlsx
+++ b/Listado ART.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\Descarga_Alicuota_ART\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F73693E-103B-403D-9EA0-E93EDF10EA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797CEF9E-712E-41C1-AFFA-08FBA02E5C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1856,8 +1856,8 @@
   <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="F2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1955,8 +1955,8 @@
         <v>18</v>
       </c>
       <c r="J2" s="2" t="str">
-        <f ca="1">CONCATENATE(TEXT(A2,"0")," - ","ART - ",TEXT(F2,"AAAAMMDD")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
-        <v>0 - ART - 20230602 - 20000000000 - Cliente</v>
+        <f ca="1">CONCATENATE(TEXT(A2,"0")," - ","ART - ",YEAR(F2)&amp;TEXT(MONTH(F2),"00")&amp;TEXT(DAY(F2),"00")," - ",SUBSTITUTE(D2,"-","")," - ",B2)</f>
+        <v>0 - ART - 20230702 - 20000000000 - Cliente</v>
       </c>
       <c r="K2" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J2,[1]Control!$A:$C,3,0),"")</f>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F66" ca="1" si="6">TODAY()</f>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -2015,8 +2015,8 @@
         <v>19</v>
       </c>
       <c r="J3" s="2" t="str">
-        <f t="shared" ref="J3:J66" ca="1" si="7">CONCATENATE(TEXT(A3,"0")," - ","ART - ",TEXT(F3,"AAAAMMDD")," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
-        <v>0 - ART - 20230602 - 20000000000 - Cliente</v>
+        <f t="shared" ref="J3:J66" ca="1" si="7">CONCATENATE(TEXT(A3,"0")," - ","ART - ",YEAR(F3)&amp;TEXT(MONTH(F3),"00")&amp;TEXT(DAY(F3),"00")," - ",SUBSTITUTE(D3,"-","")," - ",B3)</f>
+        <v>0 - ART - 20230702 - 20000000000 - Cliente</v>
       </c>
       <c r="K3" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J3,[1]Control!$A:$C,3,0),"")</f>
@@ -2066,14 +2066,14 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K4" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J4,[1]Control!$A:$C,3,0),"")</f>
@@ -2123,14 +2123,14 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K5" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J5,[1]Control!$A:$C,3,0),"")</f>
@@ -2180,14 +2180,14 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K6" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J6,[1]Control!$A:$C,3,0),"")</f>
@@ -2237,14 +2237,14 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K7" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J7,[1]Control!$A:$C,3,0),"")</f>
@@ -2294,14 +2294,14 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K8" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J8,[1]Control!$A:$C,3,0),"")</f>
@@ -2351,14 +2351,14 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K9" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J9,[1]Control!$A:$C,3,0),"")</f>
@@ -2408,14 +2408,14 @@
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K10" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J10,[1]Control!$A:$C,3,0),"")</f>
@@ -2465,14 +2465,14 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K11" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J11,[1]Control!$A:$C,3,0),"")</f>
@@ -2522,14 +2522,14 @@
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K12" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J12,[1]Control!$A:$C,3,0),"")</f>
@@ -2579,14 +2579,14 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K13" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J13,[1]Control!$A:$C,3,0),"")</f>
@@ -2636,14 +2636,14 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K14" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J14,[1]Control!$A:$C,3,0),"")</f>
@@ -2693,14 +2693,14 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K15" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J15,[1]Control!$A:$C,3,0),"")</f>
@@ -2750,14 +2750,14 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K16" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J16,[1]Control!$A:$C,3,0),"")</f>
@@ -2807,14 +2807,14 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K17" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J17,[1]Control!$A:$C,3,0),"")</f>
@@ -2864,14 +2864,14 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K18" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J18,[1]Control!$A:$C,3,0),"")</f>
@@ -2921,14 +2921,14 @@
       </c>
       <c r="F19" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K19" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J19,[1]Control!$A:$C,3,0),"")</f>
@@ -2978,14 +2978,14 @@
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K20" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J20,[1]Control!$A:$C,3,0),"")</f>
@@ -3035,14 +3035,14 @@
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K21" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J21,[1]Control!$A:$C,3,0),"")</f>
@@ -3092,14 +3092,14 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K22" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J22,[1]Control!$A:$C,3,0),"")</f>
@@ -3149,14 +3149,14 @@
       </c>
       <c r="F23" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K23" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J23,[1]Control!$A:$C,3,0),"")</f>
@@ -3206,14 +3206,14 @@
       </c>
       <c r="F24" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K24" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J24,[1]Control!$A:$C,3,0),"")</f>
@@ -3263,14 +3263,14 @@
       </c>
       <c r="F25" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K25" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J25,[1]Control!$A:$C,3,0),"")</f>
@@ -3320,14 +3320,14 @@
       </c>
       <c r="F26" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K26" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J26,[1]Control!$A:$C,3,0),"")</f>
@@ -3377,14 +3377,14 @@
       </c>
       <c r="F27" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K27" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J27,[1]Control!$A:$C,3,0),"")</f>
@@ -3434,14 +3434,14 @@
       </c>
       <c r="F28" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K28" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J28,[1]Control!$A:$C,3,0),"")</f>
@@ -3491,14 +3491,14 @@
       </c>
       <c r="F29" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K29" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J29,[1]Control!$A:$C,3,0),"")</f>
@@ -3548,14 +3548,14 @@
       </c>
       <c r="F30" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K30" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J30,[1]Control!$A:$C,3,0),"")</f>
@@ -3605,14 +3605,14 @@
       </c>
       <c r="F31" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K31" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J31,[1]Control!$A:$C,3,0),"")</f>
@@ -3662,14 +3662,14 @@
       </c>
       <c r="F32" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K32" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J32,[1]Control!$A:$C,3,0),"")</f>
@@ -3719,14 +3719,14 @@
       </c>
       <c r="F33" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K33" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J33,[1]Control!$A:$C,3,0),"")</f>
@@ -3776,14 +3776,14 @@
       </c>
       <c r="F34" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K34" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J34,[1]Control!$A:$C,3,0),"")</f>
@@ -3833,14 +3833,14 @@
       </c>
       <c r="F35" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K35" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J35,[1]Control!$A:$C,3,0),"")</f>
@@ -3890,14 +3890,14 @@
       </c>
       <c r="F36" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K36" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J36,[1]Control!$A:$C,3,0),"")</f>
@@ -3947,14 +3947,14 @@
       </c>
       <c r="F37" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K37" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J37,[1]Control!$A:$C,3,0),"")</f>
@@ -4004,14 +4004,14 @@
       </c>
       <c r="F38" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K38" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J38,[1]Control!$A:$C,3,0),"")</f>
@@ -4061,14 +4061,14 @@
       </c>
       <c r="F39" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K39" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J39,[1]Control!$A:$C,3,0),"")</f>
@@ -4118,14 +4118,14 @@
       </c>
       <c r="F40" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K40" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J40,[1]Control!$A:$C,3,0),"")</f>
@@ -4175,14 +4175,14 @@
       </c>
       <c r="F41" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K41" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J41,[1]Control!$A:$C,3,0),"")</f>
@@ -4232,14 +4232,14 @@
       </c>
       <c r="F42" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K42" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J42,[1]Control!$A:$C,3,0),"")</f>
@@ -4289,14 +4289,14 @@
       </c>
       <c r="F43" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K43" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J43,[1]Control!$A:$C,3,0),"")</f>
@@ -4346,14 +4346,14 @@
       </c>
       <c r="F44" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K44" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J44,[1]Control!$A:$C,3,0),"")</f>
@@ -4403,14 +4403,14 @@
       </c>
       <c r="F45" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K45" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J45,[1]Control!$A:$C,3,0),"")</f>
@@ -4460,14 +4460,14 @@
       </c>
       <c r="F46" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K46" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J46,[1]Control!$A:$C,3,0),"")</f>
@@ -4517,14 +4517,14 @@
       </c>
       <c r="F47" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K47" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J47,[1]Control!$A:$C,3,0),"")</f>
@@ -4574,14 +4574,14 @@
       </c>
       <c r="F48" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K48" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J48,[1]Control!$A:$C,3,0),"")</f>
@@ -4631,14 +4631,14 @@
       </c>
       <c r="F49" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K49" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J49,[1]Control!$A:$C,3,0),"")</f>
@@ -4688,14 +4688,14 @@
       </c>
       <c r="F50" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K50" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J50,[1]Control!$A:$C,3,0),"")</f>
@@ -4745,14 +4745,14 @@
       </c>
       <c r="F51" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K51" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J51,[1]Control!$A:$C,3,0),"")</f>
@@ -4802,14 +4802,14 @@
       </c>
       <c r="F52" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K52" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J52,[1]Control!$A:$C,3,0),"")</f>
@@ -4859,14 +4859,14 @@
       </c>
       <c r="F53" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K53" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J53,[1]Control!$A:$C,3,0),"")</f>
@@ -4916,14 +4916,14 @@
       </c>
       <c r="F54" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K54" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J54,[1]Control!$A:$C,3,0),"")</f>
@@ -4973,14 +4973,14 @@
       </c>
       <c r="F55" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K55" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J55,[1]Control!$A:$C,3,0),"")</f>
@@ -5030,14 +5030,14 @@
       </c>
       <c r="F56" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K56" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J56,[1]Control!$A:$C,3,0),"")</f>
@@ -5087,14 +5087,14 @@
       </c>
       <c r="F57" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K57" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J57,[1]Control!$A:$C,3,0),"")</f>
@@ -5144,14 +5144,14 @@
       </c>
       <c r="F58" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K58" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J58,[1]Control!$A:$C,3,0),"")</f>
@@ -5201,14 +5201,14 @@
       </c>
       <c r="F59" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K59" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J59,[1]Control!$A:$C,3,0),"")</f>
@@ -5258,14 +5258,14 @@
       </c>
       <c r="F60" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K60" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J60,[1]Control!$A:$C,3,0),"")</f>
@@ -5315,14 +5315,14 @@
       </c>
       <c r="F61" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K61" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J61,[1]Control!$A:$C,3,0),"")</f>
@@ -5372,14 +5372,14 @@
       </c>
       <c r="F62" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K62" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J62,[1]Control!$A:$C,3,0),"")</f>
@@ -5429,14 +5429,14 @@
       </c>
       <c r="F63" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K63" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J63,[1]Control!$A:$C,3,0),"")</f>
@@ -5486,14 +5486,14 @@
       </c>
       <c r="F64" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="J64" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K64" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J64,[1]Control!$A:$C,3,0),"")</f>
@@ -5543,14 +5543,14 @@
       </c>
       <c r="F65" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K65" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J65,[1]Control!$A:$C,3,0),"")</f>
@@ -5600,14 +5600,14 @@
       </c>
       <c r="F66" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="2" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K66" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J66,[1]Control!$A:$C,3,0),"")</f>
@@ -5618,7 +5618,7 @@
         <v/>
       </c>
       <c r="M66" s="5" t="str">
-        <f t="shared" ref="M66:M97" si="14">IF(EXACT(L66,E66),"ü","x")</f>
+        <f t="shared" ref="M66:M71" si="14">IF(EXACT(L66,E66),"ü","x")</f>
         <v>x</v>
       </c>
       <c r="N66" s="4">
@@ -5657,14 +5657,14 @@
       </c>
       <c r="F67" s="3">
         <f t="shared" ref="F67:F101" ca="1" si="17">TODAY()</f>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="2" t="str">
-        <f t="shared" ref="J67:J69" ca="1" si="18">CONCATENATE(TEXT(A67,"0")," - ","ART - ",TEXT(F67,"AAAAMMDD")," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ref="J67:J101" ca="1" si="18">CONCATENATE(TEXT(A67,"0")," - ","ART - ",YEAR(F67)&amp;TEXT(MONTH(F67),"00")&amp;TEXT(DAY(F67),"00")," - ",SUBSTITUTE(D67,"-","")," - ",B67)</f>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K67" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J67,[1]Control!$A:$C,3,0),"")</f>
@@ -5714,14 +5714,14 @@
       </c>
       <c r="F68" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="2" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K68" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J68,[1]Control!$A:$C,3,0),"")</f>
@@ -5771,14 +5771,14 @@
       </c>
       <c r="F69" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="2" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K69" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J69,[1]Control!$A:$C,3,0),"")</f>
@@ -5828,14 +5828,14 @@
       </c>
       <c r="F70" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="2" t="str">
-        <f t="shared" ref="J70:J71" ca="1" si="22">CONCATENATE(TEXT(A70,"0")," - ","ART - ",TEXT(F70,"AAAAMMDD")," - ",SUBSTITUTE(D70,"-","")," - ",B70)</f>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K70" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J70,[1]Control!$A:$C,3,0),"")</f>
@@ -5854,15 +5854,15 @@
         <v>70</v>
       </c>
       <c r="O70" s="4">
-        <f t="shared" ref="O70:O71" si="23">IF(C70=C69,1,0)</f>
+        <f t="shared" ref="O70:O71" si="22">IF(C70=C69,1,0)</f>
         <v>1</v>
       </c>
       <c r="P70" s="4">
-        <f t="shared" ref="P70:P71" si="24">IF(C70=C71,1,0)</f>
+        <f t="shared" ref="P70:P71" si="23">IF(C70=C71,1,0)</f>
         <v>1</v>
       </c>
       <c r="Q70" s="4">
-        <f t="shared" ref="Q70:Q71" si="25">SUM(O70:P70)</f>
+        <f t="shared" ref="Q70:Q71" si="24">SUM(O70:P70)</f>
         <v>2</v>
       </c>
     </row>
@@ -5885,14 +5885,14 @@
       </c>
       <c r="F71" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="J71" s="2" t="str">
-        <f t="shared" ca="1" si="22"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K71" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J71,[1]Control!$A:$C,3,0),"")</f>
@@ -5911,21 +5911,21 @@
         <v>71</v>
       </c>
       <c r="O71" s="4">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="P71" s="4">
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="P71" s="4">
+      <c r="Q71" s="4">
         <f t="shared" si="24"/>
-        <v>1</v>
-      </c>
-      <c r="Q71" s="4">
-        <f t="shared" si="25"/>
         <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="str">
-        <f t="shared" ref="A72:A101" si="26">RIGHT(D72,1)</f>
+        <f t="shared" ref="A72:A101" si="25">RIGHT(D72,1)</f>
         <v>0</v>
       </c>
       <c r="B72" t="s">
@@ -5942,14 +5942,14 @@
       </c>
       <c r="F72" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="J72" s="2" t="str">
-        <f t="shared" ref="J72:J101" ca="1" si="27">CONCATENATE(TEXT(A72,"0")," - ","ART - ",TEXT(F72,"AAAAMMDD")," - ",SUBSTITUTE(D72,"-","")," - ",B72)</f>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K72" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J72,[1]Control!$A:$C,3,0),"")</f>
@@ -5960,29 +5960,29 @@
         <v/>
       </c>
       <c r="M72" s="5" t="str">
-        <f t="shared" ref="M72:M101" si="28">IF(EXACT(L72,E72),"ü","x")</f>
+        <f t="shared" ref="M72:M101" si="26">IF(EXACT(L72,E72),"ü","x")</f>
         <v>x</v>
       </c>
       <c r="N72" s="4">
-        <f t="shared" ref="N72:N101" si="29">ROW(A72)</f>
+        <f t="shared" ref="N72:N101" si="27">ROW(A72)</f>
         <v>72</v>
       </c>
       <c r="O72" s="4">
-        <f t="shared" ref="O72:O101" si="30">IF(C72=C71,1,0)</f>
+        <f t="shared" ref="O72:O101" si="28">IF(C72=C71,1,0)</f>
         <v>1</v>
       </c>
       <c r="P72" s="4">
-        <f t="shared" ref="P72:P101" si="31">IF(C72=C73,1,0)</f>
+        <f t="shared" ref="P72:P101" si="29">IF(C72=C73,1,0)</f>
         <v>1</v>
       </c>
       <c r="Q72" s="4">
-        <f t="shared" ref="Q72:Q101" si="32">SUM(O72:P72)</f>
+        <f t="shared" ref="Q72:Q101" si="30">SUM(O72:P72)</f>
         <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B73" t="s">
@@ -5999,14 +5999,14 @@
       </c>
       <c r="F73" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K73" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J73,[1]Control!$A:$C,3,0),"")</f>
@@ -6017,29 +6017,29 @@
         <v/>
       </c>
       <c r="M73" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N73" s="4">
+        <f t="shared" si="27"/>
+        <v>73</v>
+      </c>
+      <c r="O73" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N73" s="4">
+        <v>1</v>
+      </c>
+      <c r="P73" s="4">
         <f t="shared" si="29"/>
-        <v>73</v>
-      </c>
-      <c r="O73" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P73" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q73" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B74" t="s">
@@ -6056,14 +6056,14 @@
       </c>
       <c r="F74" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="J74" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K74" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J74,[1]Control!$A:$C,3,0),"")</f>
@@ -6074,29 +6074,29 @@
         <v/>
       </c>
       <c r="M74" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N74" s="4">
+        <f t="shared" si="27"/>
+        <v>74</v>
+      </c>
+      <c r="O74" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N74" s="4">
+        <v>1</v>
+      </c>
+      <c r="P74" s="4">
         <f t="shared" si="29"/>
-        <v>74</v>
-      </c>
-      <c r="O74" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P74" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q74" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B75" t="s">
@@ -6113,14 +6113,14 @@
       </c>
       <c r="F75" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
       <c r="J75" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K75" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J75,[1]Control!$A:$C,3,0),"")</f>
@@ -6131,29 +6131,29 @@
         <v/>
       </c>
       <c r="M75" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N75" s="4">
+        <f t="shared" si="27"/>
+        <v>75</v>
+      </c>
+      <c r="O75" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N75" s="4">
+        <v>1</v>
+      </c>
+      <c r="P75" s="4">
         <f t="shared" si="29"/>
-        <v>75</v>
-      </c>
-      <c r="O75" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P75" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q75" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B76" t="s">
@@ -6170,14 +6170,14 @@
       </c>
       <c r="F76" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="J76" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K76" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J76,[1]Control!$A:$C,3,0),"")</f>
@@ -6188,29 +6188,29 @@
         <v/>
       </c>
       <c r="M76" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N76" s="4">
+        <f t="shared" si="27"/>
+        <v>76</v>
+      </c>
+      <c r="O76" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N76" s="4">
+        <v>1</v>
+      </c>
+      <c r="P76" s="4">
         <f t="shared" si="29"/>
-        <v>76</v>
-      </c>
-      <c r="O76" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P76" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q76" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B77" t="s">
@@ -6227,14 +6227,14 @@
       </c>
       <c r="F77" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
       <c r="J77" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K77" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J77,[1]Control!$A:$C,3,0),"")</f>
@@ -6245,29 +6245,29 @@
         <v/>
       </c>
       <c r="M77" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N77" s="4">
+        <f t="shared" si="27"/>
+        <v>77</v>
+      </c>
+      <c r="O77" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N77" s="4">
+        <v>1</v>
+      </c>
+      <c r="P77" s="4">
         <f t="shared" si="29"/>
-        <v>77</v>
-      </c>
-      <c r="O77" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q77" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P77" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q77" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B78" t="s">
@@ -6284,14 +6284,14 @@
       </c>
       <c r="F78" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
       <c r="J78" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K78" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J78,[1]Control!$A:$C,3,0),"")</f>
@@ -6302,29 +6302,29 @@
         <v/>
       </c>
       <c r="M78" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N78" s="4">
+        <f t="shared" si="27"/>
+        <v>78</v>
+      </c>
+      <c r="O78" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N78" s="4">
+        <v>1</v>
+      </c>
+      <c r="P78" s="4">
         <f t="shared" si="29"/>
-        <v>78</v>
-      </c>
-      <c r="O78" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q78" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P78" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q78" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B79" t="s">
@@ -6341,14 +6341,14 @@
       </c>
       <c r="F79" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K79" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J79,[1]Control!$A:$C,3,0),"")</f>
@@ -6359,29 +6359,29 @@
         <v/>
       </c>
       <c r="M79" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N79" s="4">
+        <f t="shared" si="27"/>
+        <v>79</v>
+      </c>
+      <c r="O79" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N79" s="4">
+        <v>1</v>
+      </c>
+      <c r="P79" s="4">
         <f t="shared" si="29"/>
-        <v>79</v>
-      </c>
-      <c r="O79" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q79" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P79" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q79" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B80" t="s">
@@ -6398,14 +6398,14 @@
       </c>
       <c r="F80" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="J80" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K80" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J80,[1]Control!$A:$C,3,0),"")</f>
@@ -6416,29 +6416,29 @@
         <v/>
       </c>
       <c r="M80" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N80" s="4">
+        <f t="shared" si="27"/>
+        <v>80</v>
+      </c>
+      <c r="O80" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N80" s="4">
+        <v>1</v>
+      </c>
+      <c r="P80" s="4">
         <f t="shared" si="29"/>
-        <v>80</v>
-      </c>
-      <c r="O80" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q80" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P80" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q80" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B81" t="s">
@@ -6455,14 +6455,14 @@
       </c>
       <c r="F81" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
       <c r="J81" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K81" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J81,[1]Control!$A:$C,3,0),"")</f>
@@ -6473,29 +6473,29 @@
         <v/>
       </c>
       <c r="M81" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N81" s="4">
+        <f t="shared" si="27"/>
+        <v>81</v>
+      </c>
+      <c r="O81" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N81" s="4">
+        <v>1</v>
+      </c>
+      <c r="P81" s="4">
         <f t="shared" si="29"/>
-        <v>81</v>
-      </c>
-      <c r="O81" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q81" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P81" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q81" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B82" t="s">
@@ -6512,14 +6512,14 @@
       </c>
       <c r="F82" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
       <c r="J82" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K82" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J82,[1]Control!$A:$C,3,0),"")</f>
@@ -6530,29 +6530,29 @@
         <v/>
       </c>
       <c r="M82" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N82" s="4">
+        <f t="shared" si="27"/>
+        <v>82</v>
+      </c>
+      <c r="O82" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N82" s="4">
+        <v>1</v>
+      </c>
+      <c r="P82" s="4">
         <f t="shared" si="29"/>
-        <v>82</v>
-      </c>
-      <c r="O82" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q82" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P82" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q82" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B83" t="s">
@@ -6569,14 +6569,14 @@
       </c>
       <c r="F83" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K83" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J83,[1]Control!$A:$C,3,0),"")</f>
@@ -6587,29 +6587,29 @@
         <v/>
       </c>
       <c r="M83" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N83" s="4">
+        <f t="shared" si="27"/>
+        <v>83</v>
+      </c>
+      <c r="O83" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N83" s="4">
+        <v>1</v>
+      </c>
+      <c r="P83" s="4">
         <f t="shared" si="29"/>
-        <v>83</v>
-      </c>
-      <c r="O83" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q83" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P83" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q83" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B84" t="s">
@@ -6626,14 +6626,14 @@
       </c>
       <c r="F84" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
       <c r="J84" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K84" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J84,[1]Control!$A:$C,3,0),"")</f>
@@ -6644,29 +6644,29 @@
         <v/>
       </c>
       <c r="M84" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N84" s="4">
+        <f t="shared" si="27"/>
+        <v>84</v>
+      </c>
+      <c r="O84" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N84" s="4">
+        <v>1</v>
+      </c>
+      <c r="P84" s="4">
         <f t="shared" si="29"/>
-        <v>84</v>
-      </c>
-      <c r="O84" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q84" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P84" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q84" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B85" t="s">
@@ -6683,14 +6683,14 @@
       </c>
       <c r="F85" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="J85" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K85" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J85,[1]Control!$A:$C,3,0),"")</f>
@@ -6701,29 +6701,29 @@
         <v/>
       </c>
       <c r="M85" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N85" s="4">
+        <f t="shared" si="27"/>
+        <v>85</v>
+      </c>
+      <c r="O85" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N85" s="4">
+        <v>1</v>
+      </c>
+      <c r="P85" s="4">
         <f t="shared" si="29"/>
-        <v>85</v>
-      </c>
-      <c r="O85" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q85" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P85" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q85" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B86" t="s">
@@ -6740,14 +6740,14 @@
       </c>
       <c r="F86" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="J86" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K86" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J86,[1]Control!$A:$C,3,0),"")</f>
@@ -6758,29 +6758,29 @@
         <v/>
       </c>
       <c r="M86" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N86" s="4">
+        <f t="shared" si="27"/>
+        <v>86</v>
+      </c>
+      <c r="O86" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N86" s="4">
+        <v>1</v>
+      </c>
+      <c r="P86" s="4">
         <f t="shared" si="29"/>
-        <v>86</v>
-      </c>
-      <c r="O86" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q86" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P86" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q86" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B87" t="s">
@@ -6797,14 +6797,14 @@
       </c>
       <c r="F87" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
       <c r="J87" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K87" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J87,[1]Control!$A:$C,3,0),"")</f>
@@ -6815,29 +6815,29 @@
         <v/>
       </c>
       <c r="M87" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N87" s="4">
+        <f t="shared" si="27"/>
+        <v>87</v>
+      </c>
+      <c r="O87" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N87" s="4">
+        <v>1</v>
+      </c>
+      <c r="P87" s="4">
         <f t="shared" si="29"/>
-        <v>87</v>
-      </c>
-      <c r="O87" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q87" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P87" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q87" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B88" t="s">
@@ -6854,14 +6854,14 @@
       </c>
       <c r="F88" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
       <c r="J88" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K88" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J88,[1]Control!$A:$C,3,0),"")</f>
@@ -6872,29 +6872,29 @@
         <v/>
       </c>
       <c r="M88" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N88" s="4">
+        <f t="shared" si="27"/>
+        <v>88</v>
+      </c>
+      <c r="O88" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N88" s="4">
+        <v>1</v>
+      </c>
+      <c r="P88" s="4">
         <f t="shared" si="29"/>
-        <v>88</v>
-      </c>
-      <c r="O88" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q88" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P88" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q88" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B89" t="s">
@@ -6911,14 +6911,14 @@
       </c>
       <c r="F89" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
       <c r="J89" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K89" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J89,[1]Control!$A:$C,3,0),"")</f>
@@ -6929,29 +6929,29 @@
         <v/>
       </c>
       <c r="M89" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N89" s="4">
+        <f t="shared" si="27"/>
+        <v>89</v>
+      </c>
+      <c r="O89" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N89" s="4">
+        <v>1</v>
+      </c>
+      <c r="P89" s="4">
         <f t="shared" si="29"/>
-        <v>89</v>
-      </c>
-      <c r="O89" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q89" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P89" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q89" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B90" t="s">
@@ -6968,14 +6968,14 @@
       </c>
       <c r="F90" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K90" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J90,[1]Control!$A:$C,3,0),"")</f>
@@ -6986,29 +6986,29 @@
         <v/>
       </c>
       <c r="M90" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N90" s="4">
+        <f t="shared" si="27"/>
+        <v>90</v>
+      </c>
+      <c r="O90" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N90" s="4">
+        <v>1</v>
+      </c>
+      <c r="P90" s="4">
         <f t="shared" si="29"/>
-        <v>90</v>
-      </c>
-      <c r="O90" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q90" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P90" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q90" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B91" t="s">
@@ -7025,14 +7025,14 @@
       </c>
       <c r="F91" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
       <c r="J91" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K91" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J91,[1]Control!$A:$C,3,0),"")</f>
@@ -7043,29 +7043,29 @@
         <v/>
       </c>
       <c r="M91" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N91" s="4">
+        <f t="shared" si="27"/>
+        <v>91</v>
+      </c>
+      <c r="O91" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N91" s="4">
+        <v>1</v>
+      </c>
+      <c r="P91" s="4">
         <f t="shared" si="29"/>
-        <v>91</v>
-      </c>
-      <c r="O91" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q91" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P91" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q91" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B92" t="s">
@@ -7082,14 +7082,14 @@
       </c>
       <c r="F92" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="J92" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K92" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J92,[1]Control!$A:$C,3,0),"")</f>
@@ -7100,29 +7100,29 @@
         <v/>
       </c>
       <c r="M92" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N92" s="4">
+        <f t="shared" si="27"/>
+        <v>92</v>
+      </c>
+      <c r="O92" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N92" s="4">
+        <v>1</v>
+      </c>
+      <c r="P92" s="4">
         <f t="shared" si="29"/>
-        <v>92</v>
-      </c>
-      <c r="O92" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q92" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P92" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q92" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B93" t="s">
@@ -7139,14 +7139,14 @@
       </c>
       <c r="F93" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
       <c r="J93" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K93" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J93,[1]Control!$A:$C,3,0),"")</f>
@@ -7157,29 +7157,29 @@
         <v/>
       </c>
       <c r="M93" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N93" s="4">
+        <f t="shared" si="27"/>
+        <v>93</v>
+      </c>
+      <c r="O93" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N93" s="4">
+        <v>1</v>
+      </c>
+      <c r="P93" s="4">
         <f t="shared" si="29"/>
-        <v>93</v>
-      </c>
-      <c r="O93" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q93" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P93" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q93" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B94" t="s">
@@ -7196,14 +7196,14 @@
       </c>
       <c r="F94" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
       <c r="J94" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K94" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J94,[1]Control!$A:$C,3,0),"")</f>
@@ -7214,29 +7214,29 @@
         <v/>
       </c>
       <c r="M94" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N94" s="4">
+        <f t="shared" si="27"/>
+        <v>94</v>
+      </c>
+      <c r="O94" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N94" s="4">
+        <v>1</v>
+      </c>
+      <c r="P94" s="4">
         <f t="shared" si="29"/>
-        <v>94</v>
-      </c>
-      <c r="O94" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q94" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P94" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q94" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B95" t="s">
@@ -7253,14 +7253,14 @@
       </c>
       <c r="F95" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
       <c r="J95" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K95" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J95,[1]Control!$A:$C,3,0),"")</f>
@@ -7271,29 +7271,29 @@
         <v/>
       </c>
       <c r="M95" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N95" s="4">
+        <f t="shared" si="27"/>
+        <v>95</v>
+      </c>
+      <c r="O95" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N95" s="4">
+        <v>1</v>
+      </c>
+      <c r="P95" s="4">
         <f t="shared" si="29"/>
-        <v>95</v>
-      </c>
-      <c r="O95" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q95" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P95" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q95" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B96" t="s">
@@ -7310,14 +7310,14 @@
       </c>
       <c r="F96" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
       <c r="J96" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K96" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J96,[1]Control!$A:$C,3,0),"")</f>
@@ -7328,29 +7328,29 @@
         <v/>
       </c>
       <c r="M96" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N96" s="4">
+        <f t="shared" si="27"/>
+        <v>96</v>
+      </c>
+      <c r="O96" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N96" s="4">
+        <v>1</v>
+      </c>
+      <c r="P96" s="4">
         <f t="shared" si="29"/>
-        <v>96</v>
-      </c>
-      <c r="O96" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q96" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P96" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q96" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B97" t="s">
@@ -7367,14 +7367,14 @@
       </c>
       <c r="F97" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K97" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J97,[1]Control!$A:$C,3,0),"")</f>
@@ -7385,29 +7385,29 @@
         <v/>
       </c>
       <c r="M97" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N97" s="4">
+        <f t="shared" si="27"/>
+        <v>97</v>
+      </c>
+      <c r="O97" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N97" s="4">
+        <v>1</v>
+      </c>
+      <c r="P97" s="4">
         <f t="shared" si="29"/>
-        <v>97</v>
-      </c>
-      <c r="O97" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q97" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P97" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q97" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B98" t="s">
@@ -7424,14 +7424,14 @@
       </c>
       <c r="F98" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K98" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J98,[1]Control!$A:$C,3,0),"")</f>
@@ -7442,29 +7442,29 @@
         <v/>
       </c>
       <c r="M98" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N98" s="4">
+        <f t="shared" si="27"/>
+        <v>98</v>
+      </c>
+      <c r="O98" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N98" s="4">
+        <v>1</v>
+      </c>
+      <c r="P98" s="4">
         <f t="shared" si="29"/>
-        <v>98</v>
-      </c>
-      <c r="O98" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q98" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P98" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q98" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B99" t="s">
@@ -7481,14 +7481,14 @@
       </c>
       <c r="F99" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K99" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J99,[1]Control!$A:$C,3,0),"")</f>
@@ -7499,29 +7499,29 @@
         <v/>
       </c>
       <c r="M99" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N99" s="4">
+        <f t="shared" si="27"/>
+        <v>99</v>
+      </c>
+      <c r="O99" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N99" s="4">
+        <v>1</v>
+      </c>
+      <c r="P99" s="4">
         <f t="shared" si="29"/>
-        <v>99</v>
-      </c>
-      <c r="O99" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q99" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P99" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q99" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B100" t="s">
@@ -7538,14 +7538,14 @@
       </c>
       <c r="F100" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
       <c r="J100" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K100" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J100,[1]Control!$A:$C,3,0),"")</f>
@@ -7556,29 +7556,29 @@
         <v/>
       </c>
       <c r="M100" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N100" s="4">
+        <f t="shared" si="27"/>
+        <v>100</v>
+      </c>
+      <c r="O100" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N100" s="4">
+        <v>1</v>
+      </c>
+      <c r="P100" s="4">
         <f t="shared" si="29"/>
-        <v>100</v>
-      </c>
-      <c r="O100" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q100" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P100" s="4">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="Q100" s="4">
-        <f t="shared" si="32"/>
         <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="B101" t="s">
@@ -7595,14 +7595,14 @@
       </c>
       <c r="F101" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>45079</v>
+        <v>45109</v>
       </c>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
       <c r="J101" s="2" t="str">
-        <f t="shared" ca="1" si="27"/>
-        <v>0 - ART - 20230602 - 30000000000 - Cliente</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>0 - ART - 20230702 - 30000000000 - Cliente</v>
       </c>
       <c r="K101" s="5" t="str">
         <f ca="1">IFERROR(VLOOKUP(J101,[1]Control!$A:$C,3,0),"")</f>
@@ -7613,23 +7613,23 @@
         <v/>
       </c>
       <c r="M101" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>x</v>
+      </c>
+      <c r="N101" s="4">
+        <f t="shared" si="27"/>
+        <v>101</v>
+      </c>
+      <c r="O101" s="4">
         <f t="shared" si="28"/>
-        <v>x</v>
-      </c>
-      <c r="N101" s="4">
+        <v>1</v>
+      </c>
+      <c r="P101" s="4">
         <f t="shared" si="29"/>
-        <v>101</v>
-      </c>
-      <c r="O101" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q101" s="4">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="P101" s="4">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="Q101" s="4">
-        <f t="shared" si="32"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>